<commit_message>
Working program processing from RAM
Working FIFO from RAM, timing (timers adjusted, demo program tested),
implemented QUANTUMSERVER (with inner ServerState struct), enhanced LED
on-off functions to avoid multiple invocations of driverlib with
asserts.
</commit_message>
<xml_diff>
--- a/docs/Hangulatvilágítás.xlsx
+++ b/docs/Hangulatvilágítás.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Fényprogram-protokoll" sheetId="1" r:id="rId1"/>
     <sheet name="Fénykvantum-előállítás" sheetId="2" r:id="rId2"/>
-    <sheet name="Implementációs kompromisszumok" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t>LED1</t>
   </si>
@@ -76,9 +75,6 @@
     <t>30000 egység * 100ms, ez 50 perc megjelenítésére elég. Legfelső bit = interpoláció a következőig. Ez így tömörített helyfoglalás.</t>
   </si>
   <si>
-    <t>Ilyenkor lekéri a program a következő megjelenítendő színhármas színkódját, és lineáris interpolációs végez a két szín között a tartási idő alatt.</t>
-  </si>
-  <si>
     <t>Effektív méret</t>
   </si>
   <si>
@@ -229,12 +225,6 @@
     <t>Programok közötti szünetek hossza. Maximum 60 min, legalább 1 sec. Mivel statikus, így ha 0, nem változik, egyébként íródik az érték. 4095sec lehetne az elméleti maximum, de 60 min = 3600 sec, így ez a maximális értéke a mezőnek. Hibára lehet ellenőrizni.</t>
   </si>
   <si>
-    <t>Színkvantum</t>
-  </si>
-  <si>
-    <t>500kHz</t>
-  </si>
-  <si>
     <t>Hz</t>
   </si>
   <si>
@@ -245,6 +235,24 @@
   </si>
   <si>
     <t>Villogásdetektálási frek.</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Out of date</t>
+  </si>
+  <si>
+    <t>Színváltoztatási idő</t>
+  </si>
+  <si>
+    <t>Színiterációs minimum</t>
+  </si>
+  <si>
+    <t>Színiterációs frekvencia</t>
+  </si>
+  <si>
+    <t>Ilyenkor lekéri a program a következő megjelenítendő színhármas színkódját, és lineáris interpolációt végez a két szín között a tartási idő alatt.</t>
   </si>
 </sst>
 </file>
@@ -270,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,18 +311,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -322,11 +324,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,19 +449,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -662,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +767,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="8"/>
     </row>
@@ -693,7 +785,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -821,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -846,7 +938,7 @@
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12">
@@ -854,12 +946,12 @@
         <v>11</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="8"/>
     </row>
@@ -877,18 +969,18 @@
         <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -896,16 +988,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -913,16 +1005,16 @@
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -930,13 +1022,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -944,16 +1036,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -961,7 +1053,7 @@
     </row>
     <row r="32" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="12">
@@ -969,18 +1061,18 @@
         <v>8</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -992,7 +1084,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37">
         <v>4096</v>
@@ -1004,14 +1096,14 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38">
         <f>SUM(E36:E37)</f>
         <v>45064</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1020,7 +1112,7 @@
         <v>44.0078125</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1031,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,55 +1137,55 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1">
         <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <f>B3/B2</f>
         <v>2.56</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1101,156 +1193,206 @@
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <f>1/(B7*0.001)</f>
         <v>250</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="19" t="s">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="16">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="C12" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12">
+        <f>1/(B12*1000)</f>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="E12" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="22">
+      <c r="I12" s="22"/>
+      <c r="J12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="16" t="s">
+      <c r="L12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="17" t="s">
-        <v>52</v>
-      </c>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="25"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I14" s="22"/>
+      <c r="J14" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J14" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="10">
         <f>B12*1000 / 255</f>
         <v>196.07843137254903</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <f>1/B15</f>
+        <v>5.0999999999999995E-3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16">
         <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+        <v>66</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="25"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <f>D15*1000</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <f>1000/B20</f>
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="I9:M9"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1">
-        <f>1/500 * 256</f>
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Example for lightprogram xml and xsd, corrections in architecture xlsx
Still missing a schema qualifier for xml, and a brainstorm for program
storage
</commit_message>
<xml_diff>
--- a/docs/Hangulatvilágítás.xlsx
+++ b/docs/Hangulatvilágítás.xlsx
@@ -63,9 +63,6 @@
     <t>Tartási idő (interpoláció hossza)</t>
   </si>
   <si>
-    <t>Min. 100ms, Max. 5min</t>
-  </si>
-  <si>
     <t>0x7FFF</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Ilyenkor lekéri a program a következő megjelenítendő színhármas színkódját, és lineáris interpolációt végez a két szín között a tartási idő alatt.</t>
+  </si>
+  <si>
+    <t>Min. 100ms, Max. 50min</t>
   </si>
 </sst>
 </file>
@@ -466,10 +466,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,7 +767,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="8"/>
     </row>
@@ -782,10 +782,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -924,13 +924,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="19" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="12">
@@ -946,12 +946,12 @@
         <v>11</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="8"/>
     </row>
@@ -966,21 +966,21 @@
         <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -988,16 +988,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1005,16 +1005,16 @@
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1022,13 +1022,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1036,16 +1036,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="32" spans="1:6" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="12">
@@ -1061,18 +1061,18 @@
         <v>8</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>4096</v>
@@ -1096,14 +1096,14 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E38">
         <f>SUM(E36:E37)</f>
         <v>45064</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1112,7 +1112,7 @@
         <v>44.0078125</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1137,55 +1137,55 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1">
         <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <f>B3/B2</f>
         <v>2.56</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1193,40 +1193,40 @@
         <v>0.25</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <f>1/(B7*0.001)</f>
         <v>250</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I9" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
+      <c r="I9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I10" s="17"/>
@@ -1237,109 +1237,109 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="21" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="16">
         <v>50</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <f>1/(B12*1000)</f>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K12" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="24" t="s">
         <v>50</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I13" s="22"/>
-      <c r="J13" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
+      <c r="J13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
       <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I14" s="22"/>
-      <c r="J14" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
+      <c r="J14" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="10">
         <f>B12*1000 / 255</f>
         <v>196.07843137254903</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <f>1/B15</f>
         <v>5.0999999999999995E-3</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="22"/>
-      <c r="J15" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
+      <c r="J15" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16">
         <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" s="22"/>
-      <c r="J16" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
+      <c r="J16" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1351,37 +1351,37 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19">
         <f>D15*1000</f>
         <v>5.0999999999999996</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20">
         <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21">
         <f>1000/B20</f>
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interpolation works + basic communication with PC
Interpolation works, test for interpolation verified, basic
communication just to prove the connection was established is working.
</commit_message>
<xml_diff>
--- a/docs/Hangulatvilágítás.xlsx
+++ b/docs/Hangulatvilágítás.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fényprogram-protokoll" sheetId="1" r:id="rId1"/>
     <sheet name="Fénykvantum-előállítás" sheetId="2" r:id="rId2"/>
+    <sheet name="Soros protokoll" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>LED1</t>
   </si>
@@ -253,6 +254,57 @@
   </si>
   <si>
     <t>Min. 100ms, Max. 50min</t>
+  </si>
+  <si>
+    <t>Üzenettípus</t>
+  </si>
+  <si>
+    <t>Formátum</t>
+  </si>
+  <si>
+    <t>"HEADER [headerbytes]"</t>
+  </si>
+  <si>
+    <t>Tartalom</t>
+  </si>
+  <si>
+    <t>Bájtfolyamként a programheader</t>
+  </si>
+  <si>
+    <t>"Q [quantumbytes]</t>
+  </si>
+  <si>
+    <t>Bájtfolyamként a kvantum</t>
+  </si>
+  <si>
+    <t>Kvantum</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>"START"</t>
+  </si>
+  <si>
+    <t>"STOP"</t>
+  </si>
+  <si>
+    <t>Új program leküldésének inicializálása</t>
+  </si>
+  <si>
+    <t>Programleküldés vége</t>
+  </si>
+  <si>
+    <t>Futtatás</t>
+  </si>
+  <si>
+    <t>Szövegként a futtatandó program ID-je</t>
+  </si>
+  <si>
+    <t>"RUN [ID]"</t>
   </si>
 </sst>
 </file>
@@ -754,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,4 +1447,90 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>